<commit_message>
Added two new columns for POSMasterfile table
</commit_message>
<xml_diff>
--- a/public/storage/excel-templates/POSMasterfile_template.xlsx
+++ b/public/storage/excel-templates/POSMasterfile_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\laravel\david\public\storage\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A392EA-21FF-4ACC-A1A2-059075006E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2940AE16-476B-4077-B6B8-A7E525A59F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{328A6185-D780-4165-91A9-ADA02F578883}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Item Code</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>Party Platters</t>
+  </si>
+  <si>
+    <t>DeliveryPrice</t>
+  </si>
+  <si>
+    <t>TableVibePrice</t>
   </si>
 </sst>
 </file>
@@ -145,7 +151,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -168,12 +174,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -189,6 +204,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -504,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1DBD691-EBE9-40EE-98CE-E546F90C74A6}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,10 +533,11 @@
     <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -536,11 +553,17 @@
       <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -556,11 +579,13 @@
       <c r="E2" s="4">
         <v>395</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="5"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -576,11 +601,13 @@
       <c r="E3" s="4">
         <v>925</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="5"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -596,11 +623,13 @@
       <c r="E4" s="4">
         <v>195</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="5"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -616,11 +645,13 @@
       <c r="E5" s="4">
         <v>465</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="5"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -636,11 +667,13 @@
       <c r="E6" s="4">
         <v>1495</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="5"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -656,7 +689,9 @@
       <c r="E7" s="4">
         <v>1795</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="5"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="5">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed Ticket 35 to complete newly included columns in POSMasterfile
</commit_message>
<xml_diff>
--- a/public/storage/excel-templates/POSMasterfile_template.xlsx
+++ b/public/storage/excel-templates/POSMasterfile_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\laravel\david\public\storage\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2940AE16-476B-4077-B6B8-A7E525A59F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70513D3-3260-4257-AFC8-B004327C841F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{328A6185-D780-4165-91A9-ADA02F578883}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>Item Code</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>TableVibePrice</t>
+  </si>
+  <si>
+    <t>POS Name</t>
   </si>
 </sst>
 </file>
@@ -520,24 +523,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1DBD691-EBE9-40EE-98CE-E546F90C74A6}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -545,25 +549,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -571,21 +578,24 @@
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="4">
+      <c r="F2" s="4">
         <v>395</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="5">
+      <c r="G2" s="5"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -593,21 +603,24 @@
         <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="4">
         <v>925</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="5">
+      <c r="G3" s="5"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -615,21 +628,24 @@
         <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="4">
         <v>195</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="5">
+      <c r="G4" s="5"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -637,21 +653,24 @@
         <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="4">
         <v>465</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="5">
+      <c r="G5" s="5"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -659,21 +678,24 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="4">
+      <c r="F6" s="4">
         <v>1495</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="5">
+      <c r="G6" s="5"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -681,17 +703,20 @@
         <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="4">
+      <c r="F7" s="4">
         <v>1795</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="5">
+      <c r="G7" s="5"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="5">
         <v>1</v>
       </c>
     </row>

</xml_diff>